<commit_message>
feat: Sort final report by fulfillment date
This commit introduces a change to the sorting logic of the final report as requested by the user.

- **Date Propagation:** The `Fulfilled at` date is now propagated from the order's header row to all of its associated line items. This ensures that every row has a consistent date for accurate sorting.
- **New Sort Order:** The final DataFrame is now sorted primarily by the `Fulfilled at` column in chronological order, and secondarily by the `Name` column. This presents the data in the order it was fulfilled while keeping individual order items grouped together.
</commit_message>
<xml_diff>
--- a/filtered_orders_2025-08-19_2025-08-19.xlsx
+++ b/filtered_orders_2025-08-19_2025-08-19.xlsx
@@ -483,12 +483,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>#131439</t>
+          <t>#131433</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:34 +0300</t>
+          <t>2025-08-19 12:21:01 +0300</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0334-002-XS</t>
+          <t>01-DM-0286-065-M</t>
         </is>
       </c>
       <c r="E2" s="3" t="n">
@@ -511,12 +511,12 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>#131438</t>
+          <t>#131430</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:24 +0300</t>
+          <t>2025-08-19 12:21:02 +0300</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0379-110-XL</t>
+          <t>01-DM-0185-001-XS</t>
         </is>
       </c>
       <c r="E3" s="3" t="n">
@@ -539,12 +539,12 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>#131437</t>
+          <t>#131423</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:44 +0300</t>
+          <t>2025-08-19 12:21:03 +0300</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -554,47 +554,59 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>01-TE-0375-001-L</t>
+          <t>01-DM-0372-001-L</t>
         </is>
       </c>
       <c r="E4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>#131437</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" s="4" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>01-DM-0379-110-XL</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>#131431</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:03 +0300</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0274-001-L</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>#131437</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
+          <t>#131431</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:03 +0300</t>
+        </is>
+      </c>
       <c r="C6" s="4" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>01-DM-0334-001-XL</t>
+          <t>01-DM-0226-002-L</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -607,62 +619,66 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>#131437</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>#131431</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:03 +0300</t>
+        </is>
+      </c>
       <c r="C7" s="4" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>01-TE-0373-001-L</t>
+          <t>01-DM-0185-001-L</t>
         </is>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>#131436</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:45 +0300</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>2.99</v>
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>#131431</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:03 +0300</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>01-DM-0274-002-L</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>#131436</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
+          <t>#131431</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:03 +0300</t>
+        </is>
+      </c>
       <c r="C9" s="4" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>01-DM-0379-110-L</t>
+          <t>01-DM-0288-002-L</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -675,12 +691,12 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>#131435</t>
+          <t>#131422</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 13:01:13 +0300</t>
+          <t>2025-08-19 12:21:04 +0300</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
@@ -690,81 +706,73 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0372-001-M</t>
+          <t>01-TE-0375-001-L</t>
         </is>
       </c>
       <c r="E10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="3" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>#131422</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:04 +0300</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>01-DM-0371-001-L</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
         <v>109</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>#131434</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:23 +0300</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0379-110-M</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3" t="n">
-        <v>109</v>
-      </c>
-    </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>#131433</t>
-        </is>
-      </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:21:01 +0300</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0286-065-M</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3" t="n">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>#131422</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:04 +0300</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>01-DM-0372-065-L</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>#131432</t>
+          <t>#131414</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:24 +0300</t>
+          <t>2025-08-19 12:21:05 +0300</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
@@ -774,7 +782,7 @@
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0226-001-M</t>
+          <t>01-DM-0379-110-XS</t>
         </is>
       </c>
       <c r="E13" s="3" t="n">
@@ -785,84 +793,100 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>#131431</t>
-        </is>
-      </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:21:03 +0300</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>#131414</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:05 +0300</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>01-TE-0373-001-M</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>#131416</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:05 +0300</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>fulfilled</t>
         </is>
       </c>
-      <c r="D14" s="3" t="inlineStr">
+      <c r="D15" s="3" t="inlineStr">
         <is>
           <t>01-DM-0274-001-L</t>
         </is>
       </c>
-      <c r="E14" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3" t="n">
+      <c r="E15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="n">
         <v>109</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t>#131431</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" s="4" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>01-DM-0226-002-L</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>109</v>
-      </c>
-    </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>#131431</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" s="4" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>01-DM-0185-001-L</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>109</v>
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>#131409</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:06 +0300</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>2.99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>#131431</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
+          <t>#131409</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:06 +0300</t>
+        </is>
+      </c>
       <c r="C17" s="4" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>01-DM-0274-002-L</t>
+          <t>01-DM-0289-001-XS</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -873,62 +897,66 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>#131431</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" s="4" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>01-DM-0288-002-L</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" t="n">
-        <v>109</v>
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>#131412</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:06 +0300</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>2.99</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>#131430</t>
-        </is>
-      </c>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:21:02 +0300</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0185-001-XS</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="n">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>#131412</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:21:06 +0300</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>01-DM-0286-001-XS</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>#131429</t>
+          <t>#131413</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:34 +0300</t>
+          <t>2025-08-19 12:22:14 +0300</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
@@ -938,47 +966,59 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0379-110-S</t>
+          <t>01-DM-0343-001-L</t>
         </is>
       </c>
       <c r="E20" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
-        <is>
-          <t>#131429</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" s="4" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>01-DM-0371-001-XS</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" t="n">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>#131424</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:23:18 +0300</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0290-001-L</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>#131429</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
+          <t>#131424</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:23:18 +0300</t>
+        </is>
+      </c>
       <c r="C22" s="4" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>01-DM-0377-111-XS</t>
+          <t>01-DM-0286-065-L</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1022,7 +1062,11 @@
           <t>#131428</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:24:53 +0300</t>
+        </is>
+      </c>
       <c r="C24" s="4" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
@@ -1042,7 +1086,11 @@
           <t>#131428</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:24:53 +0300</t>
+        </is>
+      </c>
       <c r="C25" s="4" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
@@ -1059,12 +1107,12 @@
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>#131427</t>
+          <t>#131426</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:34 +0300</t>
+          <t>2025-08-19 12:58:23 +0300</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
@@ -1074,45 +1122,53 @@
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>01-DM-0379-110-M</t>
         </is>
       </c>
       <c r="E26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="3" t="n">
-        <v>2.99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="inlineStr">
-        <is>
-          <t>#131427</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" s="4" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>01-DM-0185-001-M</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" t="n">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>#131434</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:23 +0300</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0379-110-M</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>#131426</t>
+          <t>#131417</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:23 +0300</t>
+          <t>2025-08-19 12:58:24 +0300</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
@@ -1122,7 +1178,7 @@
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0379-110-M</t>
+          <t>01-DM-0371-001-L</t>
         </is>
       </c>
       <c r="E28" s="3" t="n">
@@ -1135,12 +1191,12 @@
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>#131425</t>
+          <t>#131418</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:35 +0300</t>
+          <t>2025-08-19 12:58:24 +0300</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
@@ -1150,73 +1206,77 @@
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0372-065-XL</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="n">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>#131418</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:24 +0300</t>
+        </is>
+      </c>
+      <c r="C30" s="4" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>01-DM-0379-110-L</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="n">
         <v>109</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>#131424</t>
-        </is>
-      </c>
-      <c r="B30" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:23:18 +0300</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>#131419</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:24 +0300</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
         <is>
           <t>fulfilled</t>
         </is>
       </c>
-      <c r="D30" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0290-001-L</t>
-        </is>
-      </c>
-      <c r="E30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="inlineStr">
-        <is>
-          <t>#131424</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" s="4" t="inlineStr"/>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>01-DM-0286-065-L</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" t="n">
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0379-110-S</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>#131423</t>
+          <t>#131420</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:21:03 +0300</t>
+          <t>2025-08-19 12:58:24 +0300</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
@@ -1226,93 +1286,105 @@
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0372-001-L</t>
+          <t>01-DM-0185-006-M</t>
         </is>
       </c>
       <c r="E32" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>#131422</t>
-        </is>
-      </c>
-      <c r="B33" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:21:04 +0300</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="inlineStr">
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>#131420</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:24 +0300</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>01-DM-0185-001-XS</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>#131432</t>
+        </is>
+      </c>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:24 +0300</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
         <is>
           <t>fulfilled</t>
         </is>
       </c>
-      <c r="D33" s="3" t="inlineStr">
-        <is>
-          <t>01-TE-0375-001-L</t>
-        </is>
-      </c>
-      <c r="E33" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="inlineStr">
-        <is>
-          <t>#131422</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" s="4" t="inlineStr"/>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>01-DM-0371-001-L</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" t="n">
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0226-001-M</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="inlineStr">
-        <is>
-          <t>#131422</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" s="4" t="inlineStr"/>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>01-DM-0372-065-L</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" t="n">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>#131438</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:24 +0300</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0379-110-XL</t>
+        </is>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>#131421</t>
+          <t>#131407</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 13:01:14 +0300</t>
+          <t>2025-08-19 12:58:25 +0300</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
@@ -1322,67 +1394,83 @@
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>01-HD-0352-107-M</t>
+          <t>01-DM-0379-110-M</t>
         </is>
       </c>
       <c r="E36" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="3" t="n">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="inlineStr">
-        <is>
-          <t>#131421</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" s="4" t="inlineStr"/>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>01-TE-0375-001-M</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>1</v>
-      </c>
-      <c r="F37" t="n">
-        <v>59</v>
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0333-065-M</t>
+        </is>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>#131421</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr"/>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
       <c r="C38" s="4" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>01-SP-0353-107-S</t>
+          <t>01-TE-0373-001-M</t>
         </is>
       </c>
       <c r="E38" t="n">
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>#131421</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr"/>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
       <c r="C39" s="4" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>01-DM-0339-006-S</t>
+          <t>01-DM-0371-002-S</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1395,14 +1483,18 @@
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>#131421</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr"/>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
       <c r="C40" s="4" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>01-DM-0372-001-S</t>
+          <t>01-DM-0371-001-M</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1415,14 +1507,18 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>#131421</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr"/>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
       <c r="C41" s="4" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>01-DM-0379-110-S</t>
+          <t>01-DM-0372-065-M</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1435,156 +1531,160 @@
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>#131421</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
       <c r="C42" s="4" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>01-JR-0344-015-M</t>
+          <t>01-DM-0372-001-S</t>
         </is>
       </c>
       <c r="E42" t="n">
         <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>70</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="inlineStr">
-        <is>
-          <t>#131420</t>
-        </is>
-      </c>
-      <c r="B43" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:24 +0300</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D43" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0185-006-M</t>
-        </is>
-      </c>
-      <c r="E43" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F43" s="3" t="n">
-        <v>109</v>
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>01-TE-0376-001-S</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>#131420</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr"/>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
       <c r="C44" s="4" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>01-DM-0185-001-XS</t>
+          <t>01-TE-0375-001-S</t>
         </is>
       </c>
       <c r="E44" t="n">
         <v>1</v>
       </c>
       <c r="F44" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="inlineStr">
+        <is>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>01-TE-0374-001-S</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="inlineStr">
+        <is>
+          <t>#131361</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
+      <c r="C46" s="4" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>01-DM-0379-110-M</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" t="n">
         <v>109</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="inlineStr">
-        <is>
-          <t>#131419</t>
-        </is>
-      </c>
-      <c r="B45" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:24 +0300</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="inlineStr">
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>#131415</t>
+        </is>
+      </c>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
         <is>
           <t>fulfilled</t>
         </is>
       </c>
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0379-110-S</t>
-        </is>
-      </c>
-      <c r="E45" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="3" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="inlineStr">
-        <is>
-          <t>#131418</t>
-        </is>
-      </c>
-      <c r="B46" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:24 +0300</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
-      </c>
-      <c r="E46" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" s="3" t="n">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="4" t="inlineStr">
-        <is>
-          <t>#131418</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" s="4" t="inlineStr"/>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>01-DM-0379-110-L</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" t="n">
-        <v>109</v>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>01-JO-0086-001-XL</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>#131417</t>
+          <t>#131427</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:58:24 +0300</t>
+          <t>2025-08-19 12:58:34 +0300</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
@@ -1594,48 +1694,44 @@
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0371-001-L</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E48" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F48" s="3" t="n">
-        <v>109</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="inlineStr">
-        <is>
-          <t>#131416</t>
-        </is>
-      </c>
-      <c r="B49" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:21:05 +0300</t>
-        </is>
-      </c>
-      <c r="C49" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0274-001-L</t>
-        </is>
-      </c>
-      <c r="E49" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" s="3" t="n">
+      <c r="A49" s="4" t="inlineStr">
+        <is>
+          <t>#131427</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
+      <c r="C49" s="4" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>01-DM-0185-001-M</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>#131415</t>
+          <t>#131429</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1650,73 +1746,73 @@
       </c>
       <c r="D50" s="3" t="inlineStr">
         <is>
-          <t>01-JO-0086-001-XL</t>
+          <t>01-DM-0379-110-S</t>
         </is>
       </c>
       <c r="E50" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="n">
-        <v>65</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="inlineStr">
-        <is>
-          <t>#131414</t>
-        </is>
-      </c>
-      <c r="B51" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:21:05 +0300</t>
-        </is>
-      </c>
-      <c r="C51" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0379-110-XS</t>
-        </is>
-      </c>
-      <c r="E51" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3" t="n">
+      <c r="A51" s="4" t="inlineStr">
+        <is>
+          <t>#131429</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>01-DM-0371-001-XS</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>#131414</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr"/>
+          <t>#131429</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:34 +0300</t>
+        </is>
+      </c>
       <c r="C52" s="4" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>01-TE-0373-001-M</t>
+          <t>01-DM-0377-111-XS</t>
         </is>
       </c>
       <c r="E52" t="n">
         <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>#131413</t>
+          <t>#131439</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:22:14 +0300</t>
+          <t>2025-08-19 12:58:34 +0300</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr">
@@ -1726,25 +1822,25 @@
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>01-DM-0343-001-L</t>
+          <t>01-DM-0334-002-XS</t>
         </is>
       </c>
       <c r="E53" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F53" s="3" t="n">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>#131412</t>
+          <t>#131408</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 12:21:06 +0300</t>
+          <t>2025-08-19 12:58:35 +0300</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
@@ -1754,27 +1850,31 @@
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>01-TE-0373-001-M</t>
         </is>
       </c>
       <c r="E54" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F54" s="3" t="n">
-        <v>2.99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>#131412</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
+          <t>#131408</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:35 +0300</t>
+        </is>
+      </c>
       <c r="C55" s="4" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>01-DM-0286-001-XS</t>
+          <t>01-DM-0289-001-S</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1785,152 +1885,172 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="inlineStr">
-        <is>
-          <t>#131411</t>
-        </is>
-      </c>
-      <c r="B56" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 13:01:03 +0300</t>
-        </is>
-      </c>
-      <c r="C56" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="inlineStr">
-        <is>
-          <t>01-PT-0338-036-XS</t>
-        </is>
-      </c>
-      <c r="E56" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F56" s="3" t="n">
-        <v>99</v>
+      <c r="A56" s="4" t="inlineStr">
+        <is>
+          <t>#131408</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:35 +0300</t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>01-DM-0378-063-S</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>#131411</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
+          <t>#131408</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:35 +0300</t>
+        </is>
+      </c>
       <c r="C57" s="4" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>01-JK-0339-036-XL</t>
+          <t>01-PT-0239-036-S</t>
         </is>
       </c>
       <c r="E57" t="n">
         <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>99</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="4" t="inlineStr">
         <is>
-          <t>#131411</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr"/>
+          <t>#131408</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:35 +0300</t>
+        </is>
+      </c>
       <c r="C58" s="4" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>01-PT-0355-076-XL</t>
+          <t>01-DM-0185-001-M</t>
         </is>
       </c>
       <c r="E58" t="n">
         <v>1</v>
       </c>
       <c r="F58" t="n">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="inlineStr">
-        <is>
-          <t>#131411</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" s="4" t="inlineStr"/>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>01-DM-0288-002-XL</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
-        <v>1</v>
-      </c>
-      <c r="F59" t="n">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>#131425</t>
+        </is>
+      </c>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:35 +0300</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0372-065-XL</t>
+        </is>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="inlineStr">
-        <is>
-          <t>#131411</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" s="4" t="inlineStr"/>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>01-PT-0338-036-XL</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
-        <v>1</v>
-      </c>
-      <c r="F60" t="n">
-        <v>99</v>
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>#131437</t>
+        </is>
+      </c>
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:44 +0300</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D60" s="3" t="inlineStr">
+        <is>
+          <t>01-TE-0375-001-L</t>
+        </is>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="inlineStr">
-        <is>
-          <t>#131410</t>
-        </is>
-      </c>
-      <c r="B61" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 13:01:03 +0300</t>
-        </is>
-      </c>
-      <c r="C61" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="inlineStr">
-        <is>
-          <t>01-JO-0086-065-XS</t>
-        </is>
-      </c>
-      <c r="E61" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F61" s="3" t="n">
-        <v>65</v>
+      <c r="A61" s="4" t="inlineStr">
+        <is>
+          <t>#131437</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:44 +0300</t>
+        </is>
+      </c>
+      <c r="C61" s="4" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>01-DM-0379-110-XL</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="4" t="inlineStr">
         <is>
-          <t>#131410</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
+          <t>#131437</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:44 +0300</t>
+        </is>
+      </c>
       <c r="C62" s="4" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>01-DM-0379-110-XS</t>
+          <t>01-DM-0334-001-XL</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -1941,112 +2061,124 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="inlineStr">
-        <is>
-          <t>#131409</t>
-        </is>
-      </c>
-      <c r="B63" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:21:06 +0300</t>
-        </is>
-      </c>
-      <c r="C63" s="2" t="inlineStr">
+      <c r="A63" s="4" t="inlineStr">
+        <is>
+          <t>#131437</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:44 +0300</t>
+        </is>
+      </c>
+      <c r="C63" s="4" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>01-TE-0373-001-L</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>#131406</t>
+        </is>
+      </c>
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:45 +0300</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
         <is>
           <t>fulfilled</t>
         </is>
       </c>
-      <c r="D63" s="3" t="inlineStr">
+      <c r="D64" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0288-002-XL</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
+          <t>#131406</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:45 +0300</t>
+        </is>
+      </c>
+      <c r="C65" s="4" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>01-DM-0290-002-XL</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>#131436</t>
+        </is>
+      </c>
+      <c r="B66" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:45 +0300</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D66" s="3" t="inlineStr">
         <is>
           <t>07</t>
         </is>
       </c>
-      <c r="E63" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" s="3" t="n">
+      <c r="E66" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3" t="n">
         <v>2.99</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="4" t="inlineStr">
-        <is>
-          <t>#131409</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" s="4" t="inlineStr"/>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>01-DM-0289-001-XS</t>
-        </is>
-      </c>
-      <c r="E64" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="2" t="inlineStr">
-        <is>
-          <t>#131408</t>
-        </is>
-      </c>
-      <c r="B65" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:35 +0300</t>
-        </is>
-      </c>
-      <c r="C65" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D65" s="3" t="inlineStr">
-        <is>
-          <t>01-TE-0373-001-M</t>
-        </is>
-      </c>
-      <c r="E65" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" s="3" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="4" t="inlineStr">
-        <is>
-          <t>#131408</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" s="4" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>01-DM-0289-001-S</t>
-        </is>
-      </c>
-      <c r="E66" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" t="n">
-        <v>109</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="4" t="inlineStr">
         <is>
-          <t>#131408</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr"/>
+          <t>#131436</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2025-08-19 12:58:45 +0300</t>
+        </is>
+      </c>
       <c r="C67" s="4" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>01-DM-0378-063-S</t>
+          <t>01-DM-0379-110-L</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2057,112 +2189,120 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4" t="inlineStr">
-        <is>
-          <t>#131408</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" s="4" t="inlineStr"/>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>01-PT-0239-036-S</t>
-        </is>
-      </c>
-      <c r="E68" t="n">
-        <v>1</v>
-      </c>
-      <c r="F68" t="n">
-        <v>49</v>
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>#131353</t>
+        </is>
+      </c>
+      <c r="B68" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>2.99</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="4" t="inlineStr">
         <is>
-          <t>#131408</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr"/>
+          <t>#131353</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
       <c r="C69" s="4" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>01-DM-0185-001-M</t>
+          <t>01-TE-0376-001-S</t>
         </is>
       </c>
       <c r="E69" t="n">
         <v>1</v>
       </c>
       <c r="F69" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4" t="inlineStr">
+        <is>
+          <t>#131353</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
+      <c r="C70" s="4" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>01-DM-0372-065-S</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" t="n">
         <v>109</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="2" t="inlineStr">
-        <is>
-          <t>#131407</t>
-        </is>
-      </c>
-      <c r="B70" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:25 +0300</t>
-        </is>
-      </c>
-      <c r="C70" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D70" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0379-110-M</t>
-        </is>
-      </c>
-      <c r="E70" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F70" s="3" t="n">
-        <v>109</v>
-      </c>
-    </row>
     <row r="71">
-      <c r="A71" s="2" t="inlineStr">
-        <is>
-          <t>#131406</t>
-        </is>
-      </c>
-      <c r="B71" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:45 +0300</t>
-        </is>
-      </c>
-      <c r="C71" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D71" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0288-002-XL</t>
-        </is>
-      </c>
-      <c r="E71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" s="3" t="n">
+      <c r="A71" s="4" t="inlineStr">
+        <is>
+          <t>#131353</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
+      <c r="C71" s="4" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>01-DM-0371-001-S</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>1</v>
+      </c>
+      <c r="F71" t="n">
         <v>109</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="4" t="inlineStr">
         <is>
-          <t>#131406</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
+          <t>#131353</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
       <c r="C72" s="4" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>01-DM-0290-002-XL</t>
+          <t>01-DM-0372-001-S</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -2175,12 +2315,12 @@
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>#131377</t>
+          <t>#131410</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>2025-08-19 14:27:05 +0300</t>
+          <t>2025-08-19 13:01:03 +0300</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr">
@@ -2190,115 +2330,131 @@
       </c>
       <c r="D73" s="3" t="inlineStr">
         <is>
-          <t>01-TE-0374-001-M</t>
+          <t>01-JO-0086-065-XS</t>
         </is>
       </c>
       <c r="E73" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F73" s="3" t="n">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="4" t="inlineStr">
         <is>
-          <t>#131377</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr"/>
+          <t>#131410</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
       <c r="C74" s="4" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>01-DM-0379-110-XS</t>
         </is>
       </c>
       <c r="E74" t="n">
         <v>1</v>
       </c>
       <c r="F74" t="n">
-        <v>2.99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="4" t="inlineStr">
-        <is>
-          <t>#131377</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" s="4" t="inlineStr"/>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>01-DM-0358-001-M</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>1</v>
-      </c>
-      <c r="F75" t="n">
-        <v>109</v>
+      <c r="A75" s="2" t="inlineStr">
+        <is>
+          <t>#131411</t>
+        </is>
+      </c>
+      <c r="B75" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="inlineStr">
+        <is>
+          <t>01-PT-0338-036-XS</t>
+        </is>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="inlineStr">
-        <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B76" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 12:58:34 +0300</t>
-        </is>
-      </c>
-      <c r="C76" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D76" s="3" t="inlineStr">
-        <is>
-          <t>01-DM-0333-065-M</t>
-        </is>
-      </c>
-      <c r="E76" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" s="3" t="n">
-        <v>109</v>
+      <c r="A76" s="4" t="inlineStr">
+        <is>
+          <t>#131411</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
+      <c r="C76" s="4" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>01-JK-0339-036-XL</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="4" t="inlineStr">
         <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr"/>
+          <t>#131411</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
       <c r="C77" s="4" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>01-TE-0373-001-M</t>
+          <t>01-PT-0355-076-XL</t>
         </is>
       </c>
       <c r="E77" t="n">
         <v>1</v>
       </c>
       <c r="F77" t="n">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="4" t="inlineStr">
         <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr"/>
+          <t>#131411</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
       <c r="C78" s="4" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>01-DM-0371-002-S</t>
+          <t>01-DM-0288-002-XL</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2311,74 +2467,98 @@
     <row r="79">
       <c r="A79" s="4" t="inlineStr">
         <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr"/>
+          <t>#131411</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:03 +0300</t>
+        </is>
+      </c>
       <c r="C79" s="4" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>01-DM-0371-001-M</t>
+          <t>01-PT-0338-036-XL</t>
         </is>
       </c>
       <c r="E79" t="n">
         <v>1</v>
       </c>
       <c r="F79" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>#131435</t>
+        </is>
+      </c>
+      <c r="B80" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:13 +0300</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="inlineStr">
+        <is>
+          <t>01-DM-0372-001-M</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" s="3" t="n">
         <v>109</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="4" t="inlineStr">
-        <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr"/>
-      <c r="C80" s="4" t="inlineStr"/>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>01-DM-0372-065-M</t>
-        </is>
-      </c>
-      <c r="E80" t="n">
-        <v>1</v>
-      </c>
-      <c r="F80" t="n">
-        <v>109</v>
-      </c>
-    </row>
     <row r="81">
-      <c r="A81" s="4" t="inlineStr">
-        <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" s="4" t="inlineStr"/>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>01-DM-0372-001-S</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>1</v>
-      </c>
-      <c r="F81" t="n">
-        <v>109</v>
+      <c r="A81" s="2" t="inlineStr">
+        <is>
+          <t>#131421</t>
+        </is>
+      </c>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:14 +0300</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="inlineStr">
+        <is>
+          <t>01-HD-0352-107-M</t>
+        </is>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" s="3" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="4" t="inlineStr">
         <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr"/>
+          <t>#131421</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:14 +0300</t>
+        </is>
+      </c>
       <c r="C82" s="4" t="inlineStr"/>
       <c r="D82" t="inlineStr">
         <is>
-          <t>01-TE-0376-001-S</t>
+          <t>01-TE-0375-001-M</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2391,54 +2571,66 @@
     <row r="83">
       <c r="A83" s="4" t="inlineStr">
         <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr"/>
+          <t>#131421</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:14 +0300</t>
+        </is>
+      </c>
       <c r="C83" s="4" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>01-TE-0375-001-S</t>
+          <t>01-SP-0353-107-S</t>
         </is>
       </c>
       <c r="E83" t="n">
         <v>1</v>
       </c>
       <c r="F83" t="n">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="4" t="inlineStr">
         <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr"/>
+          <t>#131421</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:14 +0300</t>
+        </is>
+      </c>
       <c r="C84" s="4" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>01-TE-0374-001-S</t>
+          <t>01-DM-0339-006-S</t>
         </is>
       </c>
       <c r="E84" t="n">
         <v>1</v>
       </c>
       <c r="F84" t="n">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="4" t="inlineStr">
         <is>
-          <t>#131361</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
+          <t>#131421</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:14 +0300</t>
+        </is>
+      </c>
       <c r="C85" s="4" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>01-DM-0379-110-M</t>
+          <t>01-DM-0372-001-S</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2449,104 +2641,120 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="inlineStr">
-        <is>
-          <t>#131353</t>
-        </is>
-      </c>
-      <c r="B86" s="3" t="inlineStr">
-        <is>
-          <t>2025-08-19 13:01:03 +0300</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="inlineStr">
-        <is>
-          <t>fulfilled</t>
-        </is>
-      </c>
-      <c r="D86" s="3" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
-      </c>
-      <c r="E86" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F86" s="3" t="n">
-        <v>2.99</v>
+      <c r="A86" s="4" t="inlineStr">
+        <is>
+          <t>#131421</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:14 +0300</t>
+        </is>
+      </c>
+      <c r="C86" s="4" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>01-DM-0379-110-S</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="4" t="inlineStr">
         <is>
-          <t>#131353</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr"/>
+          <t>#131421</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2025-08-19 13:01:14 +0300</t>
+        </is>
+      </c>
       <c r="C87" s="4" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>01-TE-0376-001-S</t>
+          <t>01-JR-0344-015-M</t>
         </is>
       </c>
       <c r="E87" t="n">
         <v>1</v>
       </c>
       <c r="F87" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>#131377</t>
+        </is>
+      </c>
+      <c r="B88" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-19 14:27:05 +0300</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>fulfilled</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="inlineStr">
+        <is>
+          <t>01-TE-0374-001-M</t>
+        </is>
+      </c>
+      <c r="E88" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" s="3" t="n">
         <v>59</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="4" t="inlineStr">
-        <is>
-          <t>#131353</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" s="4" t="inlineStr"/>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>01-DM-0372-065-S</t>
-        </is>
-      </c>
-      <c r="E88" t="n">
-        <v>1</v>
-      </c>
-      <c r="F88" t="n">
-        <v>109</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="4" t="inlineStr">
         <is>
-          <t>#131353</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr"/>
+          <t>#131377</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2025-08-19 14:27:05 +0300</t>
+        </is>
+      </c>
       <c r="C89" s="4" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>01-DM-0371-001-S</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E89" t="n">
         <v>1</v>
       </c>
       <c r="F89" t="n">
-        <v>109</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="4" t="inlineStr">
         <is>
-          <t>#131353</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr"/>
+          <t>#131377</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2025-08-19 14:27:05 +0300</t>
+        </is>
+      </c>
       <c r="C90" s="4" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>01-DM-0372-001-S</t>
+          <t>01-DM-0358-001-M</t>
         </is>
       </c>
       <c r="E90" t="n">

</xml_diff>